<commit_message>
update client list and bigger input fields
</commit_message>
<xml_diff>
--- a/pv-defiscalizare/clienti.xlsx
+++ b/pv-defiscalizare/clienti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Projects\PV Defiscalizare RBC\pv-defiscalizare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AD7674-3B3A-4BEC-AB20-DDC65FF6FEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B9F33C-540E-48B5-80CA-E29A91D61F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="2820" windowWidth="17280" windowHeight="8880" xr2:uid="{EA1693D3-9885-4ED4-85F0-F2F854290B6E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EA1693D3-9885-4ED4-85F0-F2F854290B6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="77">
   <si>
     <t>Nr_Crt</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Cod_Fiscal</t>
   </si>
   <si>
-    <t>KAUFLAND ROMANIA SCS</t>
-  </si>
-  <si>
-    <t>CAREI, STR. MIHAI VITEAZU, NR. 18</t>
-  </si>
-  <si>
     <t>RO15991149</t>
   </si>
   <si>
@@ -68,12 +62,6 @@
     <t>KPOS</t>
   </si>
   <si>
-    <t>SATU MARE, STR. CAREIULUI NR. 9</t>
-  </si>
-  <si>
-    <t>SATU MARE, STR. CORVINILOR NR. 13</t>
-  </si>
-  <si>
     <t>Aviz_Distributie</t>
   </si>
   <si>
@@ -83,12 +71,6 @@
     <t>Nume_Companie</t>
   </si>
   <si>
-    <t>LIDL DISCOUNT SRL</t>
-  </si>
-  <si>
-    <t>SATU MARE, STR. LALELEI NR. 2</t>
-  </si>
-  <si>
     <t>RO22891860</t>
   </si>
   <si>
@@ -98,7 +80,193 @@
     <t>GK LIDL</t>
   </si>
   <si>
-    <t>CAREI, STR. MIHAI VITEAZU NR 36-40</t>
+    <t>SC KAUFLAND ROMANIA SCS</t>
+  </si>
+  <si>
+    <t>SC LIDL DISCOUNT SRL</t>
+  </si>
+  <si>
+    <t>SATU MARE, STR. CAREIULUI NR. 9, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>CAREI, STR. MIHAI VITEAZU, NR. 18, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>SATU MARE, STR. CORVINILOR NR. 13, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>SATU MARE, STR. LALELEI NR. 2, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>CAREI, STR. MIHAI VITEAZU NR 36-40, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>TASNAD, STR. LACRAMIOAREI NR. 55, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>NEGRESTI-OAS, STR. VICTORIEI NR. 43-45, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>SATU MARE, STR. CAREIULUI NR. 17, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>CARREFOUR ROMANIA SA</t>
+  </si>
+  <si>
+    <t>RO11588780</t>
+  </si>
+  <si>
+    <t>18 / 01.08.2018</t>
+  </si>
+  <si>
+    <t>TP LINUX C</t>
+  </si>
+  <si>
+    <t>SC SUPECO INVESTMENT SRL</t>
+  </si>
+  <si>
+    <t>SATU MARE, STR. C.S. ANDERCO NR.1, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>RO33067767</t>
+  </si>
+  <si>
+    <t>SC REWE ROMANIA SRL / PENNY MARKET</t>
+  </si>
+  <si>
+    <t>RO13348610</t>
+  </si>
+  <si>
+    <t>30 / 03.09.2018</t>
+  </si>
+  <si>
+    <t>TASNAD, STR. LARAMIOARELOR NR.36/A, 36/B, 38, JUD. SM</t>
+  </si>
+  <si>
+    <t>SATU MARE, BLD. HENRI COANDA NR. 7, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>SATU MARE, BLD. CLOSCA NR. 47, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>SATU MARE, BLD. LUCIAN BLAGA NR. 35/B, JUD. SM</t>
+  </si>
+  <si>
+    <t>NEGRESTI-OAS, STR. VICTORIEI NR. 79, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>ARDUD, STR. STEFAN CEL MARE NR. 58, JUD. SM</t>
+  </si>
+  <si>
+    <t>SATU MARE, STR. PAULESTI NR. 73, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>CAREI, STR. IGNISULUI NR. 15, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>SC PROFI ROM FOOD SRL</t>
+  </si>
+  <si>
+    <t>ARDUD</t>
+  </si>
+  <si>
+    <t>LIVADA</t>
+  </si>
+  <si>
+    <t>SC PEPCO RETAIL SRL</t>
+  </si>
+  <si>
+    <t>AUCHAN</t>
+  </si>
+  <si>
+    <t>SHOPPING</t>
+  </si>
+  <si>
+    <t>CAREI</t>
+  </si>
+  <si>
+    <t>MEDIA GALAXY</t>
+  </si>
+  <si>
+    <t>SOMESU</t>
+  </si>
+  <si>
+    <t>SC BRICOSTORE SRL</t>
+  </si>
+  <si>
+    <t>DM DROGERIE</t>
+  </si>
+  <si>
+    <t>TEDI RETAIL SHOP SRL</t>
+  </si>
+  <si>
+    <t>SUPURU DE JOS, PIATA OBOR NR. 16, JUD. SM</t>
+  </si>
+  <si>
+    <t>RO11607939</t>
+  </si>
+  <si>
+    <t>20 / 01.08.2018</t>
+  </si>
+  <si>
+    <t>TP-LINUX P</t>
+  </si>
+  <si>
+    <t>DSTORE</t>
+  </si>
+  <si>
+    <t>LIVADA, STR. SATU MARE NR. 3, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>SATU MARE, STR. DECEBAL NR. 35, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>SAT CALINESTI-OAS NR. 19 A, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>SATU MARE, STR CAREIULUI, MAG.BL.C5, JUD. SM</t>
+  </si>
+  <si>
+    <t>SAT VAMA NR. 498, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>SATU MARE, BLD. TRAIAN NR.2, CORP B AL MAG.21, JUD. SM</t>
+  </si>
+  <si>
+    <t>ARDUD, STR. STEFAN CEL MARE NR. 30, JUD. SM</t>
+  </si>
+  <si>
+    <t>HALMEU, ST. ELIBERARII NR. 49, JUD SATU MARE</t>
+  </si>
+  <si>
+    <t>TURT, STR. CALINETE NR. 39, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>SATU MARE, AL. MILCOV BL. T6B, NR.7-8, JUD. SM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEGRESTI-OAS, </t>
+  </si>
+  <si>
+    <t>SAT BERVENI NR. 2, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>SAT SANISLAU NR. 24, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>SATU MARE, STR. RODNEI NR. 32, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>SATU MARE, STR. BRASOV NR. 4, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>SATU MARE, BLD. CLOSCA NR. 33, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>SATU MARE, STR. BRANDUSA NR. 18-20, JUD. SATU MARE</t>
+  </si>
+  <si>
+    <t>NEGRESTI-OAS, STR. PIETEI NR. 1B, INC. PIATA  AGROALIMENTARA</t>
   </si>
 </sst>
 </file>
@@ -484,19 +652,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C914FE6-C13D-417C-B351-BE52C7D5BE53}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="22.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -504,22 +673,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -527,22 +696,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -550,22 +719,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -573,22 +742,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -599,19 +768,19 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -625,16 +794,818 @@
         <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
         <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>